<commit_message>
<postprocessing> run outjobs, improve silk, adjust qty to 10 pcs
</commit_message>
<xml_diff>
--- a/asm/Pick_Place.xlsx
+++ b/asm/Pick_Place.xlsx
@@ -1,20 +1,25 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
-  <workbookPr defaultThemeVersion="124226"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr defaultThemeVersion="153222"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="30" windowWidth="20115" windowHeight="10290"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="15330" windowHeight="10020"/>
   </bookViews>
   <sheets>
     <sheet name="Pick_Place" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="152511"/>
+  <extLst>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+      <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="55">
   <si>
     <t>Designator</t>
   </si>
@@ -79,25 +84,37 @@
     <t>Header 5X2</t>
   </si>
   <si>
-    <t>ML10</t>
+    <t>ML10-FCI</t>
   </si>
   <si>
     <t>JP2</t>
   </si>
   <si>
-    <t>ML10-FCI</t>
-  </si>
-  <si>
     <t>JP3</t>
   </si>
   <si>
     <t>JP4</t>
   </si>
   <si>
-    <t>Header 2</t>
-  </si>
-  <si>
-    <t>MOLEX-705430001</t>
+    <t>Header 10</t>
+  </si>
+  <si>
+    <t>1X10</t>
+  </si>
+  <si>
+    <t>JP5</t>
+  </si>
+  <si>
+    <t>JP6</t>
+  </si>
+  <si>
+    <t>HEADER 9</t>
+  </si>
+  <si>
+    <t>1X12-NOSILK</t>
+  </si>
+  <si>
+    <t>JP7</t>
   </si>
   <si>
     <t>LD1</t>
@@ -245,6 +262,9 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
     </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
   </extLst>
 </styleSheet>
 </file>
@@ -260,39 +280,39 @@
         <a:sysClr val="window" lastClr="FFFFFF"/>
       </a:lt1>
       <a:dk2>
-        <a:srgbClr val="1F497D"/>
+        <a:srgbClr val="44546A"/>
       </a:dk2>
       <a:lt2>
-        <a:srgbClr val="EEECE1"/>
+        <a:srgbClr val="E7E6E6"/>
       </a:lt2>
       <a:accent1>
-        <a:srgbClr val="4F81BD"/>
+        <a:srgbClr val="5B9BD5"/>
       </a:accent1>
       <a:accent2>
-        <a:srgbClr val="C0504D"/>
+        <a:srgbClr val="ED7D31"/>
       </a:accent2>
       <a:accent3>
-        <a:srgbClr val="9BBB59"/>
+        <a:srgbClr val="A5A5A5"/>
       </a:accent3>
       <a:accent4>
-        <a:srgbClr val="8064A2"/>
+        <a:srgbClr val="FFC000"/>
       </a:accent4>
       <a:accent5>
-        <a:srgbClr val="4BACC6"/>
+        <a:srgbClr val="4472C4"/>
       </a:accent5>
       <a:accent6>
-        <a:srgbClr val="F79646"/>
+        <a:srgbClr val="70AD47"/>
       </a:accent6>
       <a:hlink>
-        <a:srgbClr val="0000FF"/>
+        <a:srgbClr val="0563C1"/>
       </a:hlink>
       <a:folHlink>
-        <a:srgbClr val="800080"/>
+        <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -327,7 +347,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -371,172 +391,148 @@
           <a:gsLst>
             <a:gs pos="0">
               <a:schemeClr val="phClr">
-                <a:tint val="50000"/>
-                <a:satMod val="300000"/>
+                <a:lumMod val="110000"/>
+                <a:satMod val="105000"/>
+                <a:tint val="67000"/>
               </a:schemeClr>
             </a:gs>
-            <a:gs pos="35000">
+            <a:gs pos="50000">
               <a:schemeClr val="phClr">
-                <a:tint val="37000"/>
-                <a:satMod val="300000"/>
+                <a:lumMod val="105000"/>
+                <a:satMod val="103000"/>
+                <a:tint val="73000"/>
               </a:schemeClr>
             </a:gs>
             <a:gs pos="100000">
               <a:schemeClr val="phClr">
-                <a:tint val="15000"/>
-                <a:satMod val="350000"/>
+                <a:lumMod val="105000"/>
+                <a:satMod val="109000"/>
+                <a:tint val="81000"/>
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
-          <a:lin ang="16200000" scaled="1"/>
+          <a:lin ang="5400000" scaled="0"/>
         </a:gradFill>
         <a:gradFill rotWithShape="1">
           <a:gsLst>
             <a:gs pos="0">
               <a:schemeClr val="phClr">
-                <a:shade val="51000"/>
-                <a:satMod val="130000"/>
+                <a:satMod val="103000"/>
+                <a:lumMod val="102000"/>
+                <a:tint val="94000"/>
               </a:schemeClr>
             </a:gs>
-            <a:gs pos="80000">
+            <a:gs pos="50000">
               <a:schemeClr val="phClr">
-                <a:shade val="93000"/>
-                <a:satMod val="130000"/>
+                <a:satMod val="110000"/>
+                <a:lumMod val="100000"/>
+                <a:shade val="100000"/>
               </a:schemeClr>
             </a:gs>
             <a:gs pos="100000">
               <a:schemeClr val="phClr">
-                <a:shade val="94000"/>
-                <a:satMod val="135000"/>
+                <a:lumMod val="99000"/>
+                <a:satMod val="120000"/>
+                <a:shade val="78000"/>
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
-          <a:lin ang="16200000" scaled="0"/>
+          <a:lin ang="5400000" scaled="0"/>
         </a:gradFill>
       </a:fillStyleLst>
       <a:lnStyleLst>
-        <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-          <a:solidFill>
-            <a:schemeClr val="phClr">
-              <a:shade val="95000"/>
-              <a:satMod val="105000"/>
-            </a:schemeClr>
-          </a:solidFill>
-          <a:prstDash val="solid"/>
-        </a:ln>
-        <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
         </a:ln>
-        <a:ln w="38100" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
+        </a:ln>
+        <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
         </a:ln>
       </a:lnStyleLst>
       <a:effectStyleLst>
         <a:effectStyle>
+          <a:effectLst/>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst/>
+        </a:effectStyle>
+        <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="40000" dist="20000" dir="5400000" rotWithShape="0">
+            <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
               <a:srgbClr val="000000">
-                <a:alpha val="38000"/>
+                <a:alpha val="63000"/>
               </a:srgbClr>
             </a:outerShdw>
           </a:effectLst>
-        </a:effectStyle>
-        <a:effectStyle>
-          <a:effectLst>
-            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
-              <a:srgbClr val="000000">
-                <a:alpha val="35000"/>
-              </a:srgbClr>
-            </a:outerShdw>
-          </a:effectLst>
-        </a:effectStyle>
-        <a:effectStyle>
-          <a:effectLst>
-            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
-              <a:srgbClr val="000000">
-                <a:alpha val="35000"/>
-              </a:srgbClr>
-            </a:outerShdw>
-          </a:effectLst>
-          <a:scene3d>
-            <a:camera prst="orthographicFront">
-              <a:rot lat="0" lon="0" rev="0"/>
-            </a:camera>
-            <a:lightRig rig="threePt" dir="t">
-              <a:rot lat="0" lon="0" rev="1200000"/>
-            </a:lightRig>
-          </a:scene3d>
-          <a:sp3d>
-            <a:bevelT w="63500" h="25400"/>
-          </a:sp3d>
         </a:effectStyle>
       </a:effectStyleLst>
       <a:bgFillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
         </a:solidFill>
+        <a:solidFill>
+          <a:schemeClr val="phClr">
+            <a:tint val="95000"/>
+            <a:satMod val="170000"/>
+          </a:schemeClr>
+        </a:solidFill>
         <a:gradFill rotWithShape="1">
           <a:gsLst>
             <a:gs pos="0">
               <a:schemeClr val="phClr">
-                <a:tint val="40000"/>
-                <a:satMod val="350000"/>
+                <a:tint val="93000"/>
+                <a:satMod val="150000"/>
+                <a:shade val="98000"/>
+                <a:lumMod val="102000"/>
               </a:schemeClr>
             </a:gs>
-            <a:gs pos="40000">
+            <a:gs pos="50000">
               <a:schemeClr val="phClr">
-                <a:tint val="45000"/>
-                <a:shade val="99000"/>
-                <a:satMod val="350000"/>
+                <a:tint val="98000"/>
+                <a:satMod val="130000"/>
+                <a:shade val="90000"/>
+                <a:lumMod val="103000"/>
               </a:schemeClr>
             </a:gs>
             <a:gs pos="100000">
               <a:schemeClr val="phClr">
-                <a:shade val="20000"/>
-                <a:satMod val="255000"/>
+                <a:shade val="63000"/>
+                <a:satMod val="120000"/>
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
-          <a:path path="circle">
-            <a:fillToRect l="50000" t="-80000" r="50000" b="180000"/>
-          </a:path>
-        </a:gradFill>
-        <a:gradFill rotWithShape="1">
-          <a:gsLst>
-            <a:gs pos="0">
-              <a:schemeClr val="phClr">
-                <a:tint val="80000"/>
-                <a:satMod val="300000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="100000">
-              <a:schemeClr val="phClr">
-                <a:shade val="30000"/>
-                <a:satMod val="200000"/>
-              </a:schemeClr>
-            </a:gs>
-          </a:gsLst>
-          <a:path path="circle">
-            <a:fillToRect l="50000" t="50000" r="50000" b="50000"/>
-          </a:path>
+          <a:lin ang="5400000" scaled="0"/>
         </a:gradFill>
       </a:bgFillStyleLst>
     </a:fmtScheme>
   </a:themeElements>
   <a:objectDefaults/>
   <a:extraClrSchemeLst/>
+  <a:extLst>
+    <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+    </a:ext>
+  </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C28"/>
+  <dimension ref="A1:C31"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -698,45 +694,45 @@
         <v>20</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B15" s="2" t="s">
         <v>20</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="B16" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="B16" s="2" t="s">
+      <c r="C16" s="2" t="s">
         <v>26</v>
-      </c>
-      <c r="C16" s="2" t="s">
-        <v>27</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" s="2" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="B18" s="2" t="s">
         <v>29</v>
@@ -747,7 +743,7 @@
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" s="2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B19" s="2" t="s">
         <v>29</v>
@@ -758,101 +754,134 @@
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="B20" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="B20" s="2" t="s">
-        <v>29</v>
-      </c>
       <c r="C20" s="2" t="s">
-        <v>30</v>
+        <v>34</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="B21" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="C21" s="2" t="s">
         <v>34</v>
-      </c>
-      <c r="B21" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="C21" s="2" t="s">
-        <v>36</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22" s="2" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="C22" s="2" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23" s="2" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="C23" s="2" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="B24" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="B24" s="2" t="s">
-        <v>35</v>
-      </c>
       <c r="C24" s="2" t="s">
-        <v>36</v>
+        <v>40</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="B25" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="C25" s="2" t="s">
         <v>40</v>
-      </c>
-      <c r="B25" s="2" t="s">
-        <v>41</v>
-      </c>
-      <c r="C25" s="2" t="s">
-        <v>42</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A26" s="2" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B26" s="2" t="s">
-        <v>44</v>
+        <v>39</v>
       </c>
       <c r="C26" s="2" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A27" s="2" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="B27" s="2" t="s">
-        <v>46</v>
+        <v>39</v>
       </c>
       <c r="C27" s="2" t="s">
-        <v>47</v>
+        <v>40</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A28" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="B28" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="C28" s="2" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A29" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="B29" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="B28" s="2" t="s">
+      <c r="C29" s="2" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A30" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="C28" s="2" t="s">
+      <c r="B30" s="2" t="s">
         <v>50</v>
+      </c>
+      <c r="C30" s="2" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A31" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="B31" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="C31" s="2" t="s">
+        <v>54</v>
       </c>
     </row>
   </sheetData>

</xml_diff>